<commit_message>
create report for finance statemnt in excell
</commit_message>
<xml_diff>
--- a/reports/students_report.xlsx
+++ b/reports/students_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>CIC202307000</t>
+  </si>
+  <si>
+    <t>tavoz</t>
+  </si>
+  <si>
+    <t>CIC202307009</t>
   </si>
   <si>
     <t>terence</t>
@@ -432,7 +438,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,53 +557,53 @@
         <v>17</v>
       </c>
       <c r="D6">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="E6">
         <v>15.0</v>
       </c>
       <c r="F6">
-        <v>-10.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>80.0</v>
+        <v>5.0</v>
       </c>
       <c r="E7">
-        <v>80.0</v>
+        <v>15.0</v>
       </c>
       <c r="F7">
-        <v>0.0</v>
+        <v>-10.0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8">
-        <v>5.0</v>
+        <v>80.0</v>
       </c>
       <c r="E8">
-        <v>95.0</v>
+        <v>80.0</v>
       </c>
       <c r="F8">
-        <v>-90.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -605,27 +611,27 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
       <c r="D9">
         <v>5.0</v>
       </c>
       <c r="E9">
-        <v>12.0</v>
+        <v>95.0</v>
       </c>
       <c r="F9">
-        <v>-7.0</v>
+        <v>-90.0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -634,9 +640,29 @@
         <v>5.0</v>
       </c>
       <c r="E10">
+        <v>12.0</v>
+      </c>
+      <c r="F10">
+        <v>-7.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>5.0</v>
+      </c>
+      <c r="E11">
         <v>95.0</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>-90.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix student with all its methods
</commit_message>
<xml_diff>
--- a/reports/students_report.xlsx
+++ b/reports/students_report.xlsx
@@ -15,90 +15,117 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Surname</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
+  <si>
+    <t>School Name</t>
+  </si>
+  <si>
+    <t>Address:</t>
+  </si>
+  <si>
+    <t>39 Chitsere</t>
+  </si>
+  <si>
+    <t>New Mabvuku</t>
+  </si>
+  <si>
+    <t>Harare</t>
+  </si>
+  <si>
+    <t>Phone:</t>
+  </si>
+  <si>
+    <t>'+263775923458</t>
+  </si>
+  <si>
+    <t>'+263715328408</t>
+  </si>
+  <si>
+    <t>Email:</t>
+  </si>
+  <si>
+    <t>mafurataboz@gmail.com</t>
+  </si>
+  <si>
+    <t>Report Date: September 8, 2023</t>
+  </si>
+  <si>
+    <t>Outstanding Fees Summary:   Form 6</t>
   </si>
   <si>
     <t>Student ID</t>
   </si>
   <si>
-    <t>Fees</t>
-  </si>
-  <si>
-    <t>Owed Fees</t>
-  </si>
-  <si>
-    <t>Paid Amount</t>
-  </si>
-  <si>
-    <t>mitchie</t>
-  </si>
-  <si>
-    <t>mafura</t>
-  </si>
-  <si>
-    <t>CIC202307006</t>
-  </si>
-  <si>
-    <t>tabo9</t>
-  </si>
-  <si>
-    <t>CIC202307007</t>
-  </si>
-  <si>
-    <t>tanatswa</t>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Current Fees Owed</t>
   </si>
   <si>
     <t>CIC202307004</t>
   </si>
   <si>
-    <t>Tavonga</t>
-  </si>
-  <si>
-    <t>Mafura</t>
+    <t>tanatswa mafura</t>
+  </si>
+  <si>
+    <t>$97.00</t>
   </si>
   <si>
     <t>CIC202307000</t>
   </si>
   <si>
-    <t>tavoz</t>
+    <t>Tavonga Mafura</t>
+  </si>
+  <si>
+    <t>$10.33</t>
+  </si>
+  <si>
+    <t>CIC202307002</t>
+  </si>
+  <si>
+    <t>terence mafura</t>
+  </si>
+  <si>
+    <t>$25.00</t>
   </si>
   <si>
     <t>CIC202307009</t>
   </si>
   <si>
-    <t>terence</t>
-  </si>
-  <si>
-    <t>CIC202307002</t>
-  </si>
-  <si>
-    <t>CIC202307008</t>
-  </si>
-  <si>
-    <t>Tino</t>
+    <t>testnow mafura</t>
+  </si>
+  <si>
+    <t>$90.00</t>
   </si>
   <si>
     <t>CIC202307003</t>
   </si>
   <si>
-    <t>Tinovimba</t>
-  </si>
-  <si>
-    <t>Makomheke</t>
+    <t>Tino Mafura</t>
+  </si>
+  <si>
+    <t>$105.00</t>
   </si>
   <si>
     <t>CIC202307001</t>
   </si>
   <si>
-    <t>Tinovonga</t>
+    <t>Tinovimba Makomheke</t>
+  </si>
+  <si>
+    <t>$22.00</t>
   </si>
   <si>
     <t>CIC202307005</t>
+  </si>
+  <si>
+    <t>Tinovonga Mafura</t>
+  </si>
+  <si>
+    <t>Total Amount for  Form 6:</t>
+  </si>
+  <si>
+    <t>$454.33</t>
   </si>
 </sst>
 </file>
@@ -106,7 +133,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -116,16 +143,55 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -133,12 +199,47 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,235 +539,245 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="true" style="0"/>
+    <col min="3" max="3" width="17" customWidth="true" style="0"/>
+    <col min="5" max="5" width="5" customWidth="true" style="0"/>
+    <col min="6" max="6" width="5" customWidth="true" style="0"/>
+    <col min="8" max="8" width="25" customWidth="true" style="0"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" customHeight="1" ht="30">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>5.0</v>
-      </c>
-      <c r="E2">
-        <v>69.0</v>
-      </c>
-      <c r="F2">
-        <v>-64.0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="H4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:8" customHeight="1" ht="20">
+      <c r="A5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3">
-        <v>5.0</v>
-      </c>
-      <c r="E3">
-        <v>95.0</v>
-      </c>
-      <c r="F3">
-        <v>-90.0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" customHeight="1" ht="20">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>5.0</v>
-      </c>
-      <c r="E4">
-        <v>87.0</v>
-      </c>
-      <c r="F4">
-        <v>-82.0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+      <c r="B8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H8"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5">
-        <v>5.0</v>
-      </c>
-      <c r="E5">
-        <v>13.33</v>
-      </c>
-      <c r="F5">
-        <v>-8.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6">
-        <v>15.0</v>
-      </c>
-      <c r="E6">
-        <v>15.0</v>
-      </c>
-      <c r="F6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+      <c r="H9"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7">
-        <v>5.0</v>
-      </c>
-      <c r="E7">
-        <v>15.0</v>
-      </c>
-      <c r="F7">
-        <v>-10.0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8">
-        <v>80.0</v>
-      </c>
-      <c r="E8">
-        <v>80.0</v>
-      </c>
-      <c r="F8">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="H10"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9">
-        <v>5.0</v>
-      </c>
-      <c r="E9">
-        <v>95.0</v>
-      </c>
-      <c r="F9">
-        <v>-90.0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
+      <c r="H11"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10">
-        <v>5.0</v>
-      </c>
-      <c r="E10">
-        <v>12.0</v>
-      </c>
-      <c r="F10">
-        <v>-7.0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="H12"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D11">
-        <v>5.0</v>
-      </c>
-      <c r="E11">
-        <v>95.0</v>
-      </c>
-      <c r="F11">
-        <v>-90.0</v>
-      </c>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15"/>
+    </row>
+    <row r="16" spans="1:8" customHeight="1" ht="20">
+      <c r="A16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H16"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="H17"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
   </sheetData>
+  <mergeCells>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>